<commit_message>
added r scripts for descriptives
</commit_message>
<xml_diff>
--- a/rstats/r-data/FORCE-ParticipantData-All.xlsx
+++ b/rstats/r-data/FORCE-ParticipantData-All.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\data\FORCe\inputdatabase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\projects\force-moco\rstats\r-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC7870E-FD5D-44E3-801D-A368A787D982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3450B77-E1E5-4916-B8A2-BFCBE14F931B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7344" yWindow="1032" windowWidth="15696" windowHeight="11208" xr2:uid="{16E6C7DD-13E6-4124-9394-7696C05EC47F}"/>
   </bookViews>
@@ -993,7 +993,7 @@
   <dimension ref="A1:G196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,7 +1038,7 @@
         <v>73.2</v>
       </c>
       <c r="E2">
-        <v>182.1</v>
+        <v>1.821</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1061,7 +1061,7 @@
         <v>77.400000000000006</v>
       </c>
       <c r="E3">
-        <v>175.5</v>
+        <v>1.7549999999999999</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1084,7 +1084,7 @@
         <v>77.2</v>
       </c>
       <c r="E4">
-        <v>173.5</v>
+        <v>1.7350000000000001</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1107,7 +1107,7 @@
         <v>51.6</v>
       </c>
       <c r="E5">
-        <v>171</v>
+        <v>1.71</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1130,7 +1130,7 @@
         <v>50.8</v>
       </c>
       <c r="E6">
-        <v>159</v>
+        <v>1.59</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1153,7 +1153,7 @@
         <v>73.400000000000006</v>
       </c>
       <c r="E7">
-        <v>176</v>
+        <v>1.76</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1176,7 +1176,7 @@
         <v>82.2</v>
       </c>
       <c r="E8">
-        <v>182</v>
+        <v>1.82</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1199,7 +1199,7 @@
         <v>95.2</v>
       </c>
       <c r="E9">
-        <v>187</v>
+        <v>1.87</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1222,7 +1222,7 @@
         <v>77.5</v>
       </c>
       <c r="E10">
-        <v>181</v>
+        <v>1.81</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1245,7 +1245,7 @@
         <v>65.3</v>
       </c>
       <c r="E11">
-        <v>173</v>
+        <v>1.73</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1268,7 +1268,7 @@
         <v>92</v>
       </c>
       <c r="E12">
-        <v>180</v>
+        <v>1.8</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1291,7 +1291,7 @@
         <v>82</v>
       </c>
       <c r="E13">
-        <v>180.5</v>
+        <v>1.8049999999999999</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1314,7 +1314,7 @@
         <v>80.099999999999895</v>
       </c>
       <c r="E14">
-        <v>181</v>
+        <v>1.81</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1337,7 +1337,7 @@
         <v>102.4</v>
       </c>
       <c r="E15">
-        <v>195</v>
+        <v>1.95</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1360,7 +1360,7 @@
         <v>90.2</v>
       </c>
       <c r="E16">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>103.6</v>
       </c>
       <c r="E17">
-        <v>177.5</v>
+        <v>1.7749999999999999</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1406,7 +1406,7 @@
         <v>61.8</v>
       </c>
       <c r="E18">
-        <v>164</v>
+        <v>1.64</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1429,7 +1429,7 @@
         <v>92</v>
       </c>
       <c r="E19">
-        <v>182</v>
+        <v>1.82</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1452,7 +1452,7 @@
         <v>74.5</v>
       </c>
       <c r="E20">
-        <v>172.5</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -1475,7 +1475,7 @@
         <v>71.8</v>
       </c>
       <c r="E21">
-        <v>172</v>
+        <v>1.72</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1498,7 +1498,7 @@
         <v>93</v>
       </c>
       <c r="E22">
-        <v>185.5</v>
+        <v>1.855</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1521,7 +1521,7 @@
         <v>74.599999999999895</v>
       </c>
       <c r="E23">
-        <v>185</v>
+        <v>1.85</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1544,7 +1544,7 @@
         <v>59.2</v>
       </c>
       <c r="E24">
-        <v>158</v>
+        <v>1.58</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1567,7 +1567,7 @@
         <v>53.7</v>
       </c>
       <c r="E25">
-        <v>163.5</v>
+        <v>1.635</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -1590,7 +1590,7 @@
         <v>83.7</v>
       </c>
       <c r="E26">
-        <v>180.5</v>
+        <v>1.8049999999999999</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1613,7 +1613,7 @@
         <v>100.2</v>
       </c>
       <c r="E27">
-        <v>194</v>
+        <v>1.94</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1636,7 +1636,7 @@
         <v>74.400000000000006</v>
       </c>
       <c r="E28">
-        <v>178</v>
+        <v>1.78</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1659,7 +1659,7 @@
         <v>63.8</v>
       </c>
       <c r="E29">
-        <v>172</v>
+        <v>1.72</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1682,7 +1682,7 @@
         <v>63.3</v>
       </c>
       <c r="E30">
-        <v>163</v>
+        <v>1.63</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1705,7 +1705,7 @@
         <v>83.5</v>
       </c>
       <c r="E31">
-        <v>165</v>
+        <v>1.65</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1728,7 +1728,7 @@
         <v>78.5</v>
       </c>
       <c r="E32">
-        <v>170</v>
+        <v>1.7</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1751,7 +1751,7 @@
         <v>65.3</v>
       </c>
       <c r="E33">
-        <v>165</v>
+        <v>1.65</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1774,7 +1774,7 @@
         <v>56.6</v>
       </c>
       <c r="E34">
-        <v>165</v>
+        <v>1.65</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1797,7 +1797,7 @@
         <v>67.8</v>
       </c>
       <c r="E35">
-        <v>175</v>
+        <v>1.75</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1820,7 +1820,7 @@
         <v>66.900000000000006</v>
       </c>
       <c r="E36">
-        <v>178.5</v>
+        <v>1.7849999999999999</v>
       </c>
       <c r="F36">
         <v>2</v>
@@ -1843,7 +1843,7 @@
         <v>61.8</v>
       </c>
       <c r="E37">
-        <v>164</v>
+        <v>1.64</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -1866,7 +1866,7 @@
         <v>88.5</v>
       </c>
       <c r="E38">
-        <v>191</v>
+        <v>1.91</v>
       </c>
       <c r="F38">
         <v>2</v>
@@ -1889,7 +1889,7 @@
         <v>-1</v>
       </c>
       <c r="E39">
-        <v>-1</v>
+        <v>-0.01</v>
       </c>
       <c r="F39">
         <v>2</v>
@@ -1912,7 +1912,7 @@
         <v>-1</v>
       </c>
       <c r="E40">
-        <v>-1</v>
+        <v>-0.01</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1935,7 +1935,7 @@
         <v>84</v>
       </c>
       <c r="E41">
-        <v>175</v>
+        <v>1.75</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1958,7 +1958,7 @@
         <v>92.9</v>
       </c>
       <c r="E42">
-        <v>188</v>
+        <v>1.88</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1981,7 +1981,7 @@
         <v>96.1</v>
       </c>
       <c r="E43">
-        <v>178.5</v>
+        <v>1.7849999999999999</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -2004,7 +2004,7 @@
         <v>78.599999999999895</v>
       </c>
       <c r="E44">
-        <v>183.5</v>
+        <v>1.835</v>
       </c>
       <c r="F44">
         <v>2</v>
@@ -2027,7 +2027,7 @@
         <v>88.5</v>
       </c>
       <c r="E45">
-        <v>178</v>
+        <v>1.78</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2050,7 +2050,7 @@
         <v>83</v>
       </c>
       <c r="E46">
-        <v>189.5</v>
+        <v>1.895</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2073,7 +2073,7 @@
         <v>87.7</v>
       </c>
       <c r="E47">
-        <v>192</v>
+        <v>1.92</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2096,7 +2096,7 @@
         <v>91.4</v>
       </c>
       <c r="E48">
-        <v>182.5</v>
+        <v>1.825</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -2119,7 +2119,7 @@
         <v>83</v>
       </c>
       <c r="E49">
-        <v>171</v>
+        <v>1.71</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -2142,7 +2142,7 @@
         <v>64.599999999999895</v>
       </c>
       <c r="E50">
-        <v>164</v>
+        <v>1.64</v>
       </c>
       <c r="F50">
         <v>1</v>

</xml_diff>